<commit_message>
Added "Sources found via https://www.data.va.gov/"
</commit_message>
<xml_diff>
--- a/Opioid_Data--US_Department_Of_Veterans_Affairs.xlsx
+++ b/Opioid_Data--US_Department_Of_Veterans_Affairs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Opioid_Abuse_Predictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F302C123-4606-4EED-A98A-01C799DA504E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFFCBCE-A63E-4500-B6F6-6D2F4AE1C435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="60" windowWidth="28860" windowHeight="15390" xr2:uid="{42361019-0208-45FB-AE44-63CB2E894E89}"/>
+    <workbookView xWindow="-48" yWindow="72" windowWidth="23088" windowHeight="12312" xr2:uid="{42361019-0208-45FB-AE44-63CB2E894E89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>U.S. Department of Veterans Affairs Opioid Data</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>https://www.data.va.gov/api/views/dwpj-hgp7/rows.csv?date=20230707&amp;accessType=DOWNLOAD</t>
+  </si>
+  <si>
+    <t>Sources found via https://www.data.va.gov</t>
   </si>
 </sst>
 </file>
@@ -188,11 +191,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -509,9 +511,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4D5BFAD-764A-48F6-831C-C7B82FA1A092}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -536,89 +540,77 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>31</v>
+      <c r="D9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>28</v>
+      <c r="D10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -626,49 +618,66 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D8" r:id="rId1" xr:uid="{EE2677F5-B22E-4206-B8D6-DEC994378B66}"/>
-    <hyperlink ref="E8" r:id="rId2" xr:uid="{C8A541F1-D68B-4458-BED9-611C2032F304}"/>
-    <hyperlink ref="D9" r:id="rId3" xr:uid="{78264EED-0B55-428B-A1B1-6FAC41C201D7}"/>
-    <hyperlink ref="E9" r:id="rId4" xr:uid="{5F125423-4C3E-4CDC-8EC7-E37C6F18707F}"/>
-    <hyperlink ref="D10" r:id="rId5" xr:uid="{A98AD225-3B44-4A62-A5C5-5D01B591795A}"/>
-    <hyperlink ref="E10" r:id="rId6" xr:uid="{D6F46D8E-78B7-4281-8ABD-3423E046DCD3}"/>
-    <hyperlink ref="D11" r:id="rId7" xr:uid="{C0134E51-3826-40A1-91A8-188A4D9BFA96}"/>
-    <hyperlink ref="E11" r:id="rId8" xr:uid="{BCA63280-2E37-4112-91AC-2975E055338D}"/>
-    <hyperlink ref="D12" r:id="rId9" xr:uid="{2817CBE8-A6B6-4919-8732-678BAA77BB0A}"/>
-    <hyperlink ref="E12" r:id="rId10" xr:uid="{954475D2-9679-40CB-98FC-D1EAA207D670}"/>
-    <hyperlink ref="D13" r:id="rId11" xr:uid="{06CA37A7-7F0B-49E1-BA3A-F37DC9F321BD}"/>
-    <hyperlink ref="E13" r:id="rId12" xr:uid="{37B853BC-AFDC-4404-AD8B-CA160F16CE7D}"/>
+    <hyperlink ref="D9" r:id="rId1" xr:uid="{EE2677F5-B22E-4206-B8D6-DEC994378B66}"/>
+    <hyperlink ref="E9" r:id="rId2" xr:uid="{C8A541F1-D68B-4458-BED9-611C2032F304}"/>
+    <hyperlink ref="D10" r:id="rId3" xr:uid="{78264EED-0B55-428B-A1B1-6FAC41C201D7}"/>
+    <hyperlink ref="E10" r:id="rId4" xr:uid="{5F125423-4C3E-4CDC-8EC7-E37C6F18707F}"/>
+    <hyperlink ref="D11" r:id="rId5" xr:uid="{A98AD225-3B44-4A62-A5C5-5D01B591795A}"/>
+    <hyperlink ref="E11" r:id="rId6" xr:uid="{D6F46D8E-78B7-4281-8ABD-3423E046DCD3}"/>
+    <hyperlink ref="D12" r:id="rId7" xr:uid="{C0134E51-3826-40A1-91A8-188A4D9BFA96}"/>
+    <hyperlink ref="E12" r:id="rId8" xr:uid="{BCA63280-2E37-4112-91AC-2975E055338D}"/>
+    <hyperlink ref="D13" r:id="rId9" xr:uid="{2817CBE8-A6B6-4919-8732-678BAA77BB0A}"/>
+    <hyperlink ref="E13" r:id="rId10" xr:uid="{954475D2-9679-40CB-98FC-D1EAA207D670}"/>
+    <hyperlink ref="D14" r:id="rId11" xr:uid="{06CA37A7-7F0B-49E1-BA3A-F37DC9F321BD}"/>
+    <hyperlink ref="E14" r:id="rId12" xr:uid="{37B853BC-AFDC-4404-AD8B-CA160F16CE7D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>

</xml_diff>